<commit_message>
Remove english answers in french questions file
</commit_message>
<xml_diff>
--- a/questions/QCM_Factorio_fr.xlsx
+++ b/questions/QCM_Factorio_fr.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="98">
   <si>
     <t>Questions</t>
   </si>
@@ -307,6 +307,12 @@
   </si>
   <si>
     <t>Les bâtiments inactifs ne consomment pas d'énergie.</t>
+  </si>
+  <si>
+    <t>Vrai</t>
+  </si>
+  <si>
+    <t>Faux</t>
   </si>
 </sst>
 </file>
@@ -824,7 +830,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -834,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,11 +1183,11 @@
       <c r="B12" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="20" t="b">
-        <v>0</v>
+      <c r="C12" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
@@ -1517,11 +1523,11 @@
       <c r="B24" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" s="20" t="b">
-        <v>0</v>
+      <c r="C24" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="E24" s="19"/>
       <c r="F24" s="20"/>
@@ -1542,11 +1548,11 @@
       <c r="B25" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" s="17" t="b">
-        <v>0</v>
+      <c r="C25" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="17"/>
@@ -1567,11 +1573,11 @@
       <c r="B26" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" s="20" t="b">
-        <v>0</v>
+      <c r="C26" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="20"/>

</xml_diff>

<commit_message>
Sort questions in xlsx file per difficulty
</commit_message>
<xml_diff>
--- a/questions/QCM_Factorio_fr.xlsx
+++ b/questions/QCM_Factorio_fr.xlsx
@@ -830,7 +830,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -841,7 +841,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,28 +891,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="16">
-        <v>1</v>
-      </c>
-      <c r="D2" s="17">
-        <v>2</v>
-      </c>
-      <c r="E2" s="16">
-        <v>4</v>
-      </c>
-      <c r="F2" s="17">
-        <v>8</v>
-      </c>
-      <c r="G2" s="16">
-        <v>4</v>
-      </c>
-      <c r="H2" s="17">
-        <v>4</v>
-      </c>
-      <c r="I2" s="16">
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="23">
+        <v>4</v>
+      </c>
+      <c r="H2" s="24">
+        <v>4</v>
+      </c>
+      <c r="I2" s="23">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -920,28 +920,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G3" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="22">
         <v>4</v>
       </c>
       <c r="I3" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -949,19 +949,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G4" s="21">
         <v>3</v>
@@ -970,7 +970,7 @@
         <v>4</v>
       </c>
       <c r="I4" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -978,22 +978,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H5" s="24">
         <v>4</v>
@@ -1007,22 +1007,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G6" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="22">
         <v>4</v>
@@ -1036,22 +1036,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="G7" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H7" s="24">
         <v>4</v>
@@ -1065,22 +1065,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G8" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="22">
         <v>4</v>
@@ -1094,25 +1094,21 @@
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>28</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="23">
         <v>2</v>
       </c>
       <c r="H9" s="24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I9" s="23">
         <v>1</v>
@@ -1123,25 +1119,21 @@
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>33</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I10" s="21">
         <v>1</v>
@@ -1152,98 +1144,102 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>38</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="23">
         <v>2</v>
       </c>
       <c r="H11" s="24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I11" s="23">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21">
-        <v>1</v>
-      </c>
-      <c r="H12" s="22">
-        <v>2</v>
-      </c>
-      <c r="I12" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="C12" s="19">
+        <v>1</v>
+      </c>
+      <c r="D12" s="20">
+        <v>2</v>
+      </c>
+      <c r="E12" s="19">
+        <v>4</v>
+      </c>
+      <c r="F12" s="20">
+        <v>8</v>
+      </c>
+      <c r="G12" s="19">
+        <v>4</v>
+      </c>
+      <c r="H12" s="20">
+        <v>4</v>
+      </c>
+      <c r="I12" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+        <v>23</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="G13" s="23">
         <v>2</v>
       </c>
       <c r="H13" s="24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I13" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="G14" s="21">
         <v>3</v>
@@ -1252,7 +1248,7 @@
         <v>4</v>
       </c>
       <c r="I14" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
@@ -1260,28 +1256,24 @@
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>76</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="23">
         <v>1</v>
       </c>
       <c r="H15" s="24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I15" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
@@ -1289,28 +1281,24 @@
         <v>15</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>52</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H16" s="22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I16" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
@@ -1318,22 +1306,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="G17" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H17" s="24">
         <v>4</v>
@@ -1347,22 +1335,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G18" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18" s="22">
         <v>4</v>
@@ -1376,22 +1364,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="G19" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H19" s="24">
         <v>4</v>
@@ -1405,22 +1393,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="G20" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" s="22">
         <v>4</v>
@@ -1434,22 +1422,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G21" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H21" s="24">
         <v>4</v>
@@ -1463,22 +1451,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G22" s="21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H22" s="22">
         <v>4</v>
@@ -1492,22 +1480,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G23" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H23" s="24">
         <v>4</v>
@@ -1516,82 +1504,97 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>23</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="20"/>
+        <v>81</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>69</v>
+      </c>
       <c r="G24" s="21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H24" s="22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I24" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="17"/>
+        <v>83</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>85</v>
+      </c>
       <c r="G25" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H25" s="24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I25" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <v>25</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
+        <v>89</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>90</v>
+      </c>
       <c r="G26" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H26" s="22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I26" s="21">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:I26">
+    <sortCondition ref="I2:I26"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>